<commit_message>
clear old test & run successful
</commit_message>
<xml_diff>
--- a/test1234.xlsx
+++ b/test1234.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\offic\Desktop\School\BUS 601 Fund tech\Zag2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\offic\Desktop\School\BUS 601 Fund Management\Zag2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DC4615-143B-4D66-B151-5ECDB580B7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D8703F-30F8-46FF-A78C-52FC0A42DDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7050" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,13 +38,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -55,7 +64,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -63,12 +72,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,12 +399,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="123.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C59" s="2"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C75" s="2"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C76" s="2"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C77" s="2"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C78" s="2"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C83" s="2"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C84" s="2"/>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C85" s="2"/>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C86" s="2"/>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C87" s="2"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C88" s="2"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C89" s="2"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C90" s="2"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C91" s="2"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C92" s="2"/>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C93" s="2"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C94" s="2"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C95" s="2"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C96" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>